<commit_message>
Updated Domain Management, Manage Network, IPTransit all files
</commit_message>
<xml_diff>
--- a/APTAutomationProject/src/com/saksoft/qa/datalibrary/APT_DomainManagement.xlsx
+++ b/APTAutomationProject/src/com/saksoft/qa/datalibrary/APT_DomainManagement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="119">
   <si>
     <t>ExistingOrderNumber</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Domain Management</t>
   </si>
   <si>
-    <t>Domain_</t>
-  </si>
-  <si>
     <t>ServiceEmail</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>Edit_ServiceFax</t>
   </si>
   <si>
-    <t>BR (Brazil)</t>
-  </si>
-  <si>
     <t>ExistingRFIREQNumber</t>
   </si>
   <si>
@@ -258,112 +252,130 @@
     <t>ChangeOrder_OrderNumber</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Domain_16</t>
-  </si>
-  <si>
-    <t>dmdomain16.com</t>
-  </si>
-  <si>
-    <t>domainocn16</t>
-  </si>
-  <si>
-    <t>testreference16</t>
-  </si>
-  <si>
-    <t>domaincontact16</t>
-  </si>
-  <si>
-    <t>domain16@test.com</t>
-  </si>
-  <si>
-    <t>9973899074</t>
-  </si>
-  <si>
-    <t>DomainOrder_16</t>
-  </si>
-  <si>
-    <t>DomainRFI_16</t>
-  </si>
-  <si>
-    <t>DomainService_16</t>
-  </si>
-  <si>
-    <t>domainservice_16@gmail.com</t>
-  </si>
-  <si>
-    <t>9987894934</t>
-  </si>
-  <si>
-    <t>Domainuser16</t>
-  </si>
-  <si>
-    <t>domainemail16@gmail.com</t>
-  </si>
-  <si>
-    <t>servicecomp16</t>
-  </si>
-  <si>
-    <t>546743</t>
-  </si>
-  <si>
-    <t>+49-1873-809382</t>
-  </si>
-  <si>
     <t>hfisesy@ui</t>
   </si>
   <si>
-    <t>DomainOrderedit_16</t>
-  </si>
-  <si>
-    <t>DomainRFIedit_16</t>
-  </si>
-  <si>
-    <t>DomainServiceedit_18</t>
-  </si>
-  <si>
-    <t>TestRemarksedit18</t>
-  </si>
-  <si>
-    <t>domainserviceedit_18@gmail.com</t>
-  </si>
-  <si>
-    <t>9498383983</t>
-  </si>
-  <si>
-    <t>Domainuseredit18</t>
-  </si>
-  <si>
-    <t>domainemailedit18@gmail.com</t>
-  </si>
-  <si>
-    <t>colttest18</t>
-  </si>
-  <si>
-    <t>serviceedit18</t>
-  </si>
-  <si>
-    <t>testedit18</t>
-  </si>
-  <si>
     <t>23, Mangalore</t>
   </si>
   <si>
-    <t>servicecompedit18</t>
-  </si>
-  <si>
-    <t>598446</t>
-  </si>
-  <si>
     <t>Ooty</t>
   </si>
   <si>
     <t>TN</t>
   </si>
   <si>
-    <t>+49-4773-827893</t>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>546724</t>
+  </si>
+  <si>
+    <t>0620</t>
+  </si>
+  <si>
+    <t>Domain0620</t>
+  </si>
+  <si>
+    <t>dmdomain0620.com</t>
+  </si>
+  <si>
+    <t>domainocn0620</t>
+  </si>
+  <si>
+    <t>testreference0620</t>
+  </si>
+  <si>
+    <t>domaincontact0620</t>
+  </si>
+  <si>
+    <t>domain0620@test.com</t>
+  </si>
+  <si>
+    <t>9973825582</t>
+  </si>
+  <si>
+    <t>9973857923</t>
+  </si>
+  <si>
+    <t>DomainOrder_0620</t>
+  </si>
+  <si>
+    <t>DomainRFI_0620</t>
+  </si>
+  <si>
+    <t>DomainService_0620</t>
+  </si>
+  <si>
+    <t>domainservice_0620@gmail.com</t>
+  </si>
+  <si>
+    <t>9987892672</t>
+  </si>
+  <si>
+    <t>user0620</t>
+  </si>
+  <si>
+    <t>domainemail0620@gmail.com</t>
+  </si>
+  <si>
+    <t>servicecomp0620</t>
+  </si>
+  <si>
+    <t>+49-1873-809275</t>
+  </si>
+  <si>
+    <t>+49-1873-809156</t>
+  </si>
+  <si>
+    <t>DomainServiceedit_0620</t>
+  </si>
+  <si>
+    <t>TestRemarksedit0620</t>
+  </si>
+  <si>
+    <t>domainserviceedit_0620@gmail.com</t>
+  </si>
+  <si>
+    <t>9498382368</t>
+  </si>
+  <si>
+    <t>Domainuseredit0620</t>
+  </si>
+  <si>
+    <t>domainemailedit0620@gmail.com</t>
+  </si>
+  <si>
+    <t>testedit0620</t>
+  </si>
+  <si>
+    <t>serviceedit0620</t>
+  </si>
+  <si>
+    <t>colttest0620</t>
+  </si>
+  <si>
+    <t>servicecompedit0620</t>
+  </si>
+  <si>
+    <t>598487</t>
+  </si>
+  <si>
+    <t>+49-4773-827345</t>
+  </si>
+  <si>
+    <t>+49-4773-827874</t>
+  </si>
+  <si>
+    <t>DomainOrderedit_0620</t>
+  </si>
+  <si>
+    <t>DomainRFIedit_0620</t>
   </si>
 </sst>
 </file>
@@ -720,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BF6" sqref="BF6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BK10" sqref="BK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -764,8 +776,7 @@
     <col min="43" max="59" width="9.140625" style="2"/>
     <col min="60" max="60" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="30.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="30.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="64" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -822,7 +833,7 @@
         <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>26</v>
@@ -831,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>1</v>
@@ -849,153 +860,153 @@
         <v>23</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="AH1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="AM1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="AP1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BF1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="BG1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BK1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:63">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>4</v>
@@ -1010,7 +1021,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>4</v>
@@ -1019,136 +1030,136 @@
         <v>5</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="AF2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="AH2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BG2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="BK2" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR2" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV2" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="BG2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>